<commit_message>
implemented firewall basic info class and function
created a dataframe and pass it to the class
</commit_message>
<xml_diff>
--- a/templates/workbook/firewall_deployment.xlsx
+++ b/templates/workbook/firewall_deployment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archit.desai/Documents/Automation/dev0.2/netops_v01/templates/csv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archit.desai/Documents/Automation/dev0.2/netops_v01/templates/workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82950A68-DA88-6941-9517-4B20D247E1E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF1DE71-A154-5145-ADB3-99141642F912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9540" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{136705CC-B8D5-3F4C-A3B1-A61D4279F6C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="58">
   <si>
     <t>USABD</t>
   </si>
@@ -56,39 +56,18 @@
     <t>mgmt</t>
   </si>
   <si>
-    <t>MANAGEMENT_IP</t>
-  </si>
-  <si>
-    <t>MANAGEMENT_GATEWAY</t>
-  </si>
-  <si>
-    <t>MANAGEMENT_INTERFACE</t>
-  </si>
-  <si>
     <t>MFG</t>
   </si>
   <si>
-    <t>HA_INTERFACE</t>
-  </si>
-  <si>
     <t>PORT1,PORT2</t>
   </si>
   <si>
-    <t>HA_MODE</t>
-  </si>
-  <si>
     <t>ACTIVE-PASSIVE</t>
   </si>
   <si>
-    <t>LACP_INTERFACE</t>
-  </si>
-  <si>
     <t>X1,X2</t>
   </si>
   <si>
-    <t>10.1.1.15/24, 10.1.1.16/24</t>
-  </si>
-  <si>
     <t>10.1.1.1</t>
   </si>
   <si>
@@ -101,9 +80,6 @@
     <t>10.1.6.1/24</t>
   </si>
   <si>
-    <t>DEFAULT_ROUTE</t>
-  </si>
-  <si>
     <t>10.1.2.1</t>
   </si>
   <si>
@@ -131,12 +107,6 @@
     <t>VIM PLC</t>
   </si>
   <si>
-    <t>FIELD_NAME</t>
-  </si>
-  <si>
-    <t>USER_INPUT</t>
-  </si>
-  <si>
     <t>DHCP_SERVER</t>
   </si>
   <si>
@@ -152,9 +122,6 @@
     <t>10.1.7.129/25</t>
   </si>
   <si>
-    <t>FIREWALL_MODEL</t>
-  </si>
-  <si>
     <t>200F</t>
   </si>
   <si>
@@ -179,9 +146,6 @@
     <t>27 GBPS</t>
   </si>
   <si>
-    <t>SEGMENTATION_TYPE</t>
-  </si>
-  <si>
     <t>MID END SMALL DATACENTER/DMZ/SEGMENTATION FIREWALLS</t>
   </si>
   <si>
@@ -207,13 +171,52 @@
   </si>
   <si>
     <t>FIREWALL MODELS</t>
+  </si>
+  <si>
+    <t>10.1.1.15, 10.1.1.16</t>
+  </si>
+  <si>
+    <t>FIREWALL MODEL</t>
+  </si>
+  <si>
+    <t>SEGMENTATION TYPE</t>
+  </si>
+  <si>
+    <t>MANAGEMENT INTERFACE</t>
+  </si>
+  <si>
+    <t>MANAGEMENT GATEWAY</t>
+  </si>
+  <si>
+    <t>MANAGEMENT IPS</t>
+  </si>
+  <si>
+    <t>MANAGEMENT NETMASK</t>
+  </si>
+  <si>
+    <t>HA MODE</t>
+  </si>
+  <si>
+    <t>DEFAULT ROUTE</t>
+  </si>
+  <si>
+    <t>USER INPUT</t>
+  </si>
+  <si>
+    <t>FIELD NAME</t>
+  </si>
+  <si>
+    <t>HA INTERFACES</t>
+  </si>
+  <si>
+    <t>LACP INTERFACES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -248,6 +251,14 @@
       <b/>
       <sz val="18"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -389,7 +400,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -413,6 +424,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -866,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{459C81C4-3B05-E845-B47C-E451D4556627}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11:K12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,22 +898,22 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>38</v>
+      <c r="A2" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -907,7 +921,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -915,15 +929,15 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="14" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -931,179 +945,187 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
+      <c r="A7" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
+      <c r="A8" s="14" t="s">
+        <v>50</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>35</v>
+    </row>
+    <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>401</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
+        <v>404</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>405</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1149,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1171,7 +1193,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1195,7 +1217,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1219,7 +1241,7 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -1398,7 +1420,7 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1422,7 +1444,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1446,7 +1468,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1470,7 +1492,7 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="6" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -1627,7 +1649,7 @@
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1651,7 +1673,7 @@
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="6" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1675,7 +1697,7 @@
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="6" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1699,7 +1721,7 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1723,7 +1745,7 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="6" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new update jinja2 deployment new deployment
</commit_message>
<xml_diff>
--- a/templates/workbook/firewall_deployment.xlsx
+++ b/templates/workbook/firewall_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archit.desai/Documents/Automation/dev0.2/netops_v01/templates/workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF1DE71-A154-5145-ADB3-99141642F912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9A0188-AA55-1648-AD56-203F12ACDAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9540" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{136705CC-B8D5-3F4C-A3B1-A61D4279F6C9}"/>
   </bookViews>
@@ -197,9 +197,6 @@
     <t>HA MODE</t>
   </si>
   <si>
-    <t>DEFAULT ROUTE</t>
-  </si>
-  <si>
     <t>USER INPUT</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>LACP INTERFACES</t>
+  </si>
+  <si>
+    <t>DEFAULT GATEWAY</t>
   </si>
 </sst>
 </file>
@@ -883,7 +883,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,10 +898,10 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
@@ -994,7 +994,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1002,7 +1002,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
working redirect to the individual ha mode function
</commit_message>
<xml_diff>
--- a/templates/workbook/firewall_deployment.xlsx
+++ b/templates/workbook/firewall_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/archit.desai/Documents/Automation/dev0.2/netops_v01/templates/workbook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A9A0188-AA55-1648-AD56-203F12ACDAB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EADB8AE-4E5D-4746-AA1D-B184C5A27E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-9540" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{136705CC-B8D5-3F4C-A3B1-A61D4279F6C9}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>PORT1,PORT2</t>
   </si>
   <si>
-    <t>ACTIVE-PASSIVE</t>
-  </si>
-  <si>
     <t>X1,X2</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>DEFAULT GATEWAY</t>
+  </si>
+  <si>
+    <t>a-a</t>
   </si>
 </sst>
 </file>
@@ -422,11 +422,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -883,7 +883,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -898,22 +898,22 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>46</v>
+      <c r="A2" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -921,7 +921,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
@@ -929,15 +929,15 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
-        <v>47</v>
+      <c r="A5" s="13" t="s">
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -945,85 +945,85 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
-        <v>48</v>
+      <c r="A7" s="13" t="s">
+        <v>47</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>50</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="B9" s="1">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
-        <v>49</v>
+      <c r="A10" s="13" t="s">
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>52</v>
+      <c r="A11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="14" t="s">
-        <v>55</v>
+      <c r="A12" s="13" t="s">
+        <v>54</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
-        <v>57</v>
-      </c>
       <c r="B14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>41</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1031,16 +1031,16 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1048,16 +1048,16 @@
         <v>401</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1065,16 +1065,16 @@
         <v>402</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1082,16 +1082,16 @@
         <v>403</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1099,16 +1099,16 @@
         <v>404</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1116,19 +1116,24 @@
         <v>405</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B11" xr:uid="{4A588D59-737A-E742-81A2-23038A319B00}">
+      <formula1>"a-p, a-a, standalone"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1148,28 +1153,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:20" ht="22" thickBot="1" x14ac:dyDescent="0.3">
@@ -1193,7 +1198,7 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
       <c r="T3" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1217,7 +1222,7 @@
       <c r="R4" s="3"/>
       <c r="S4" s="3"/>
       <c r="T4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1241,7 +1246,7 @@
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -1420,7 +1425,7 @@
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
       <c r="T15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1444,7 +1449,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
       <c r="T16" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1468,7 +1473,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1492,7 +1497,7 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
       <c r="T18" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
@@ -1649,7 +1654,7 @@
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
       <c r="T27" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1673,7 +1678,7 @@
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
       <c r="T28" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1697,7 +1702,7 @@
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
       <c r="T29" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1721,7 +1726,7 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
       <c r="T30" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="21" x14ac:dyDescent="0.25">
@@ -1745,7 +1750,7 @@
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
       <c r="T31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">

</xml_diff>